<commit_message>
vault backup: 2023-12-18 21:54:47
</commit_message>
<xml_diff>
--- a/8051/attachments/sound.xlsx
+++ b/8051/attachments/sound.xlsx
@@ -30,6 +30,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">频率（</t>
     </r>
@@ -38,6 +39,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hz</t>
     </r>
@@ -46,6 +48,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -56,6 +59,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">精确频率（</t>
     </r>
@@ -64,6 +68,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hz</t>
     </r>
@@ -72,6 +77,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -82,6 +88,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">周期（</t>
     </r>
@@ -90,6 +97,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">us</t>
     </r>
@@ -98,6 +106,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -108,6 +117,198 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">翻转周期（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">翻转周期取整（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">重装载值</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5#</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">（基准频率）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">6#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">音符频率呈指数增长</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">音符周期=2 * 翻转周期，一个周期需要翻转两次</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">口，实现发出对应频率的声音</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">STC89C52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">机器周期</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">，重装载值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">触发中断（计数器溢出）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">65536-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">周期</t>
     </r>
@@ -116,6 +317,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/2</t>
     </r>
@@ -124,121 +326,27 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">（</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">取整</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">实现固定周期触发两次中断，翻转两次</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">us</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">周期</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">取整（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">us</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">重装载值</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5#</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">（基准频率）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">6#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">音符频率呈指数增长</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">一个周期需要翻转两次</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">IO</t>
     </r>
@@ -247,114 +355,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">口，实现发出对应频率的声音</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">STC89C52</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">机器周期</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1us</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">，重装载值</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">触发中断（计数器溢出）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">65536-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">周期</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">取整</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">实现固定周期触发两次中断，翻转两次</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">IO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">口，发出对应频率的声音</t>
     </r>
@@ -372,6 +373,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -392,6 +394,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -436,7 +439,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,7 +452,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,17 +480,17 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.81"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1517,48 +1524,48 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
vault backup: 2023-12-19 00:04:04
</commit_message>
<xml_diff>
--- a/8051/attachments/sound.xlsx
+++ b/8051/attachments/sound.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t xml:space="preserve">音符</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">重装载值</t>
+  </si>
+  <si>
+    <t xml:space="preserve">索引</t>
   </si>
   <si>
     <t xml:space="preserve">1#</t>
@@ -368,7 +371,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -395,6 +398,11 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -439,7 +447,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,6 +457,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,20 +489,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,6 +528,9 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -543,10 +559,13 @@
         <f aca="false">65536-F2</f>
         <v>63628</v>
       </c>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>277</v>
@@ -571,6 +590,9 @@
         <f aca="false">65536-F3</f>
         <v>63731</v>
       </c>
+      <c r="H3" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -599,10 +621,13 @@
         <f aca="false">65536-F4</f>
         <v>63835</v>
       </c>
+      <c r="H4" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>311</v>
@@ -627,6 +652,9 @@
         <f aca="false">65536-F5</f>
         <v>63928</v>
       </c>
+      <c r="H5" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -655,6 +683,9 @@
         <f aca="false">65536-F6</f>
         <v>64021</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -683,10 +714,13 @@
         <f aca="false">65536-F7</f>
         <v>64103</v>
       </c>
+      <c r="H7" s="1" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>370</v>
@@ -711,6 +745,9 @@
         <f aca="false">65536-F8</f>
         <v>64185</v>
       </c>
+      <c r="H8" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -739,10 +776,13 @@
         <f aca="false">65536-F9</f>
         <v>64260</v>
       </c>
+      <c r="H9" s="1" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>415</v>
@@ -767,10 +807,13 @@
         <f aca="false">65536-F10</f>
         <v>64331</v>
       </c>
+      <c r="H10" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>440</v>
@@ -794,10 +837,13 @@
         <f aca="false">65536-F11</f>
         <v>64400</v>
       </c>
+      <c r="H11" s="1" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>466</v>
@@ -822,6 +868,9 @@
         <f aca="false">65536-F12</f>
         <v>64463</v>
       </c>
+      <c r="H12" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -850,6 +899,9 @@
         <f aca="false">65536-F13</f>
         <v>64528</v>
       </c>
+      <c r="H13" s="1" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -878,10 +930,13 @@
         <f aca="false">65536-F14</f>
         <v>64580</v>
       </c>
+      <c r="H14" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>554</v>
@@ -906,6 +961,9 @@
         <f aca="false">65536-F15</f>
         <v>64633</v>
       </c>
+      <c r="H15" s="1" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -934,10 +992,13 @@
         <f aca="false">65536-F16</f>
         <v>64684</v>
       </c>
+      <c r="H16" s="1" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>622</v>
@@ -962,6 +1023,9 @@
         <f aca="false">65536-F17</f>
         <v>64732</v>
       </c>
+      <c r="H17" s="1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -990,6 +1054,9 @@
         <f aca="false">65536-F18</f>
         <v>64777</v>
       </c>
+      <c r="H18" s="1" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1018,10 +1085,13 @@
         <f aca="false">65536-F19</f>
         <v>64820</v>
       </c>
+      <c r="H19" s="1" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>740</v>
@@ -1046,6 +1116,9 @@
         <f aca="false">65536-F20</f>
         <v>64860</v>
       </c>
+      <c r="H20" s="1" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1074,10 +1147,13 @@
         <f aca="false">65536-F21</f>
         <v>64898</v>
       </c>
+      <c r="H21" s="1" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>831</v>
@@ -1102,6 +1178,9 @@
         <f aca="false">65536-F22</f>
         <v>64934</v>
       </c>
+      <c r="H22" s="1" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1130,10 +1209,13 @@
         <f aca="false">65536-F23</f>
         <v>64968</v>
       </c>
+      <c r="H23" s="1" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>932</v>
@@ -1158,6 +1240,9 @@
         <f aca="false">65536-F24</f>
         <v>65000</v>
       </c>
+      <c r="H24" s="1" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1186,6 +1271,9 @@
         <f aca="false">65536-F25</f>
         <v>65030</v>
       </c>
+      <c r="H25" s="1" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1214,10 +1302,13 @@
         <f aca="false">65536-F26</f>
         <v>65058</v>
       </c>
+      <c r="H26" s="1" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>1109</v>
@@ -1242,6 +1333,9 @@
         <f aca="false">65536-F27</f>
         <v>65085</v>
       </c>
+      <c r="H27" s="1" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -1270,10 +1364,13 @@
         <f aca="false">65536-F28</f>
         <v>65110</v>
       </c>
+      <c r="H28" s="1" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>1245</v>
@@ -1298,6 +1395,9 @@
         <f aca="false">65536-F29</f>
         <v>65134</v>
       </c>
+      <c r="H29" s="1" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1326,6 +1426,9 @@
         <f aca="false">65536-F30</f>
         <v>65157</v>
       </c>
+      <c r="H30" s="1" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -1354,10 +1457,13 @@
         <f aca="false">65536-F31</f>
         <v>65178</v>
       </c>
+      <c r="H31" s="1" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>1480</v>
@@ -1382,6 +1488,9 @@
         <f aca="false">65536-F32</f>
         <v>65198</v>
       </c>
+      <c r="H32" s="1" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1410,10 +1519,13 @@
         <f aca="false">65536-F33</f>
         <v>65217</v>
       </c>
+      <c r="H33" s="1" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>1661</v>
@@ -1438,6 +1550,9 @@
         <f aca="false">65536-F34</f>
         <v>65235</v>
       </c>
+      <c r="H34" s="1" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1466,10 +1581,13 @@
         <f aca="false">65536-F35</f>
         <v>65252</v>
       </c>
+      <c r="H35" s="1" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>1865</v>
@@ -1494,6 +1612,9 @@
         <f aca="false">65536-F36</f>
         <v>65268</v>
       </c>
+      <c r="H36" s="1" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1522,50 +1643,53 @@
         <f aca="false">65536-F37</f>
         <v>65283</v>
       </c>
+      <c r="H37" s="1" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+      <c r="A38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A39" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>